<commit_message>
Update ug, team doc
</commit_message>
<xml_diff>
--- a/ENTRIES_ALL.xlsx
+++ b/ENTRIES_ALL.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NKC/Desktop/CS2113/budbud/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC72928-0DEC-454F-BCA3-2E3D42698F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RECORD DATA" r:id="rId3" sheetId="1"/>
-    <sheet name="SUMMARY DATA" r:id="rId4" sheetId="2"/>
+    <sheet name="RECORD DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="SUMMARY DATA" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>NAME</t>
   </si>
@@ -94,6 +102,18 @@
   </si>
   <si>
     <t xml:space="preserve">friend  ... colleague  </t>
+  </si>
+  <si>
+    <t>Payment To John</t>
+  </si>
+  <si>
+    <t>20-08-2018</t>
+  </si>
+  <si>
+    <t>Payment To Bob</t>
+  </si>
+  <si>
+    <t>20-12-2018</t>
   </si>
   <si>
     <t>INCOME</t>
@@ -108,11 +128,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -124,7 +143,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -142,16 +161,35 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:varyColors val="false"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -163,25 +201,31 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SUMMARY DATA'!$A$2:$A$7</c:f>
+              <c:f>'SUMMARY DATA'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>20-08-2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12-12-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>20-12-2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>01-01-2019</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>12-02-2019</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>20-02-2019</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>11-11-2019</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>12-12-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -189,30 +233,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SUMMARY DATA'!$B$2:$B$7</c:f>
+              <c:f>'SUMMARY DATA'!$B$2:$B$9</c:f>
               <c:numCache>
-                <c:ptCount val="6"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>200.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-52FD-694F-A472-815CAD191915}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -225,25 +282,31 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SUMMARY DATA'!$A$2:$A$7</c:f>
+              <c:f>'SUMMARY DATA'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>20-08-2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12-12-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>20-12-2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>01-01-2019</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>12-02-2019</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>20-02-2019</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>11-11-2019</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>12-12-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -251,30 +314,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SUMMARY DATA'!$C$2:$C$7</c:f>
+              <c:f>'SUMMARY DATA'!$C$2:$C$9</c:f>
               <c:numCache>
-                <c:ptCount val="6"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-52FD-694F-A472-815CAD191915}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -287,25 +363,31 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'SUMMARY DATA'!$A$2:$A$7</c:f>
+              <c:f>'SUMMARY DATA'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>20-08-2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12-12-2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>20-12-2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>01-01-2019</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>12-02-2019</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>20-02-2019</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>11-11-2019</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>12-12-2019</c:v>
                 </c:pt>
               </c:strCache>
@@ -313,31 +395,53 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SUMMARY DATA'!$D$2:$D$7</c:f>
+              <c:f>'SUMMARY DATA'!$D$2:$D$9</c:f>
               <c:numCache>
-                <c:ptCount val="6"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>200.0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.0</c:v>
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-52FD-694F-A472-815CAD191915}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="1"/>
         <c:axId val="2"/>
       </c:lineChart>
@@ -346,21 +450,27 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2"/>
         <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="2"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -371,9 +481,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="tr"/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -384,8 +496,8 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -398,18 +510,24 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Diagramm0"/>
+        <xdr:cNvPr id="2" name="Diagramm0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="8001000" cy="5715000"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -418,15 +536,318 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,242 +861,295 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
-        <v>100.0</v>
+      <c r="C2">
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="n">
-        <v>100.0</v>
+      <c r="C3">
+        <v>100</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>100.0</v>
+      <c r="C4">
+        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="n">
-        <v>100.0</v>
+      <c r="C5">
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="n">
-        <v>100.0</v>
+      <c r="C6">
+        <v>100</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="n">
-        <v>100.0</v>
+      <c r="C7">
+        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="n">
-        <v>100.0</v>
+      <c r="C8">
+        <v>100</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="n">
-        <v>-5.0</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="n">
-        <v>100.0</v>
+      <c r="C10">
+        <v>100</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>-10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>-100</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-10</v>
+      </c>
+      <c r="D2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>-100</v>
+      </c>
+      <c r="D4">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-5.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-5</v>
+      </c>
+      <c r="D7">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>300.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>100.0</v>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>